<commit_message>
C U D of TB tested, C U D of Ta updated
</commit_message>
<xml_diff>
--- a/A.xlsx
+++ b/A.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>a</t>
   </si>
@@ -49,10 +49,13 @@
     <t>ee</t>
   </si>
   <si>
-    <t>A001232</t>
+    <t>qqq</t>
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>www</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1042,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelRow="2"/>
@@ -1109,8 +1112,8 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="1">
-        <v>4522342</v>
+      <c r="A3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">

</xml_diff>

<commit_message>
calculateTc() and fuzzySearchTcByB() and exportTc()  tested
</commit_message>
<xml_diff>
--- a/A.xlsx
+++ b/A.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="13190"/>
+    <workbookView windowWidth="28800" windowHeight="13390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>a</t>
   </si>
@@ -49,13 +49,19 @@
     <t>ee</t>
   </si>
   <si>
-    <t>1qaz</t>
+    <t>A00051</t>
   </si>
   <si>
     <t>A</t>
   </si>
   <si>
-    <t>www</t>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A0005A</t>
+  </si>
+  <si>
+    <t>A0006A</t>
   </si>
 </sst>
 </file>
@@ -704,11 +710,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1039,13 +1048,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="$A5:$XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelRow="3"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
@@ -1072,31 +1081,33 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1">
-        <v>0</v>
+      <c r="G2" s="3">
+        <v>1</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -1108,36 +1119,69 @@
         <v>0</v>
       </c>
       <c r="K2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
         <v>1</v>
       </c>
       <c r="H3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>